<commit_message>
Black box table changed (small changes)
</commit_message>
<xml_diff>
--- a/ЧЯ - ЛР4.xlsx
+++ b/ЧЯ - ЛР4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16848" windowHeight="5597" firstSheet="6" activeTab="9"/>
+    <workbookView windowWidth="25600" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="Текстовое меню" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="148">
   <si>
     <t>№</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Т4</t>
+  </si>
+  <si>
+    <t>Т5</t>
   </si>
   <si>
     <t>Тесты</t>
@@ -145,11 +148,15 @@
     <t>Тип введенного значения</t>
   </si>
   <si>
-    <t>Т5</t>
-  </si>
-  <si>
     <t xml:space="preserve">find
 </t>
+  </si>
+  <si>
+    <t>{-2,-3,-1}</t>
+  </si>
+  <si>
+    <t>Введите команду или help для вывода инструкции:
+Массив должен быть отсортирован</t>
   </si>
   <si>
     <t>не число</t>
@@ -1195,55 +1202,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Запятая" xfId="1" builtinId="3"/>
-    <cellStyle name="Денежный" xfId="2" builtinId="4"/>
-    <cellStyle name="Процент" xfId="3" builtinId="5"/>
-    <cellStyle name="Запятая [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Денежный [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Гиперссылка" xfId="6" builtinId="8"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="7" builtinId="9"/>
-    <cellStyle name="Примечание" xfId="8" builtinId="10"/>
-    <cellStyle name="Предупреждающий текст" xfId="9" builtinId="11"/>
-    <cellStyle name="Заголовок" xfId="10" builtinId="15"/>
-    <cellStyle name="Пояснительный текст" xfId="11" builtinId="53"/>
-    <cellStyle name="Заголовок 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Заголовок 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Заголовок 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Заголовок 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Ввод" xfId="16" builtinId="20"/>
-    <cellStyle name="Вывод" xfId="17" builtinId="21"/>
-    <cellStyle name="Вычисление" xfId="18" builtinId="22"/>
-    <cellStyle name="Проверить ячейку" xfId="19" builtinId="23"/>
-    <cellStyle name="Связанная ячейка" xfId="20" builtinId="24"/>
-    <cellStyle name="Итого" xfId="21" builtinId="25"/>
-    <cellStyle name="Хороший" xfId="22" builtinId="26"/>
-    <cellStyle name="Плохой" xfId="23" builtinId="27"/>
-    <cellStyle name="Нейтральный" xfId="24" builtinId="28"/>
-    <cellStyle name="Акцент1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% — Акцент1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% — Акцент1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% — Акцент1" xfId="28" builtinId="32"/>
-    <cellStyle name="Акцент2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% — Акцент2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% — Акцент2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% — Акцент2" xfId="32" builtinId="36"/>
-    <cellStyle name="Акцент3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% — Акцент3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% — Акцент3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% — Акцент3" xfId="36" builtinId="40"/>
-    <cellStyle name="Акцент4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% — Акцент4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% — Акцент4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% — Акцент4" xfId="40" builtinId="44"/>
-    <cellStyle name="Акцент5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% — Акцент5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% — Акцент5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% — Акцент5" xfId="44" builtinId="48"/>
-    <cellStyle name="Акцент6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% — Акцент6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% — Акцент6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% — Акцент6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1728,13 +1735,13 @@
   <sheetPr/>
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8"/>
   <cols>
-    <col min="13" max="13" width="30.3684210526316" customWidth="1"/>
+    <col min="13" max="13" width="30.3671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1756,263 +1763,290 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" ht="26" customHeight="1" spans="10:13">
       <c r="J2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>10</v>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" ht="35" customHeight="1" spans="2:13">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>14</v>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" ht="39" customHeight="1" spans="2:13">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>19</v>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" ht="36" customHeight="1" spans="10:13">
       <c r="J5" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>22</v>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" ht="28.8" spans="2:11">
+        <v>12</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" ht="68" spans="2:13">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
       <c r="B16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
       <c r="B20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
       <c r="B23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
       <c r="B26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
+        <v>41</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
       <c r="B27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
       <c r="B30">
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:6">
@@ -2020,52 +2054,55 @@
         <v>2</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
       <c r="B39" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2079,13 +2116,13 @@
   <sheetPr/>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8"/>
   <cols>
-    <col min="13" max="13" width="24.3157894736842" customWidth="1"/>
+    <col min="13" max="13" width="24.3125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2108,124 +2145,124 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" ht="43.2" spans="2:13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="51" spans="2:13">
       <c r="B2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
         <v>2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" ht="43.2" spans="2:13">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" ht="51" spans="2:13">
       <c r="B3">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" ht="43.2" spans="2:13">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" ht="51" spans="2:13">
       <c r="B4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L4" t="s">
-        <v>134</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" ht="43.2" spans="10:13">
+        <v>136</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" ht="51" spans="10:13">
       <c r="J5" t="s">
         <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L5" t="s">
-        <v>137</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" ht="43.2" spans="2:13">
+        <v>139</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" ht="51" spans="2:13">
       <c r="B6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>140</v>
+        <v>6</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="L6" t="s">
-        <v>141</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:7">
@@ -2233,80 +2270,80 @@
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2320,11 +2357,11 @@
   <sheetPr/>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -2340,82 +2377,82 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" ht="72" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="84" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" ht="100.8" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" ht="118" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" ht="43.2" spans="2:3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="51" spans="2:3">
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" ht="43.2" spans="2:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" ht="51" spans="2:4">
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2433,7 +2470,7 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -2449,32 +2486,32 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" ht="72" spans="5:7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="84" spans="5:7">
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" ht="86.4" spans="2:7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" ht="101" spans="2:7">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -2482,36 +2519,36 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" ht="57.6" spans="2:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="68" spans="2:4">
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2529,7 +2566,7 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -2545,47 +2582,47 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" ht="57.6" spans="5:8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" ht="68" spans="5:8">
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" ht="72" spans="2:8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" ht="84" spans="2:8">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -2593,36 +2630,36 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" ht="57.6" spans="2:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" ht="68" spans="2:4">
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2636,18 +2673,18 @@
   <sheetPr/>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2659,123 +2696,123 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" ht="57.6" spans="8:11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="68" spans="8:11">
       <c r="H2" t="s">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="2:11">
       <c r="B3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="2:11">
       <c r="B4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -2783,23 +2820,23 @@
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -2807,42 +2844,42 @@
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" ht="57.6" spans="2:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" ht="68" spans="2:4">
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2860,7 +2897,7 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -2879,81 +2916,81 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" ht="86.4" spans="2:10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="101" spans="2:10">
       <c r="B2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" ht="115.2" spans="2:10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" ht="135" spans="2:10">
       <c r="B3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" ht="86.4" spans="2:10">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" ht="101" spans="2:10">
       <c r="B4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -2961,23 +2998,23 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -2985,42 +3022,42 @@
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" ht="72" spans="2:6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" ht="84" spans="2:6">
       <c r="B16" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3034,11 +3071,11 @@
   <sheetPr/>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -3054,16 +3091,16 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="7:10">
@@ -3071,30 +3108,30 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" ht="57.6" spans="2:10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" ht="68" spans="2:10">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -3102,20 +3139,20 @@
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -3123,20 +3160,20 @@
         <v>0</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -3144,20 +3181,20 @@
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -3165,36 +3202,36 @@
         <v>0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" ht="72" spans="2:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" ht="84" spans="2:5">
       <c r="B21" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3208,13 +3245,13 @@
   <sheetPr/>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8"/>
   <cols>
-    <col min="13" max="13" width="24.2631578947368" customWidth="1"/>
+    <col min="13" max="13" width="24.265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3237,161 +3274,161 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" ht="43.2" spans="10:13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="51" spans="10:13">
       <c r="J2" t="s">
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" ht="57.6" spans="2:13">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" ht="68" spans="2:13">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" ht="57.6" spans="2:13">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" ht="68" spans="2:13">
       <c r="B4">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" ht="57.6" spans="2:13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" ht="68" spans="2:13">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" ht="43.2" spans="2:13">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" ht="51" spans="2:13">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -3399,10 +3436,10 @@
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -3410,48 +3447,48 @@
         <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3465,11 +3502,11 @@
   <sheetPr/>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -3488,126 +3525,126 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" ht="86.4" spans="8:11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="101" spans="8:11">
       <c r="H2" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" ht="86.4" spans="2:11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" ht="101" spans="2:11">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" ht="86.4" spans="2:11">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" ht="101" spans="2:11">
       <c r="B4">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" ht="57.6" spans="2:6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" ht="68" spans="2:6">
       <c r="B13" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>